<commit_message>
status added for pending and done record, select many added
</commit_message>
<xml_diff>
--- a/packing_list.xlsx
+++ b/packing_list.xlsx
@@ -30,12 +30,18 @@
       <sz val="14"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
+        <bgColor rgb="00D3D3D3"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -50,11 +56,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,14 +450,290 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21-06-24</t>
-        </is>
+          <t>22-06-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Party : </t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Job Name : </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>WRP MGX KRE ROU 8TW 29G+11.8G(4008652)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>SNo.</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Roll No.</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Gross Wt.</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Tare Wt.</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Core Wt.</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>Net Wt.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="n">
+        <v>15</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>24.000</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>23.240</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>16</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>15.000</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>14.240</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="n">
+        <v>17</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>20.000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>19.240</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>59</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="F9" t="n">
+        <v>56.72</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Job Name : </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>bad vaiety</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>SNo.</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Roll No.</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Gross Wt.</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Tare Wt.</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>Core Wt.</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>Net Wt.</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="n">
+        <v>18</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>20.000</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>19.240</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>20</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>19.24</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B10:F10"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
resolved database error while reading for variety
</commit_message>
<xml_diff>
--- a/packing_list.xlsx
+++ b/packing_list.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01-07-24</t>
+          <t>16-07-24</t>
         </is>
       </c>
     </row>
@@ -462,7 +462,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>neelam</t>
+          <t>PARLE PRODUCTS</t>
         </is>
       </c>
     </row>
@@ -474,7 +474,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>WRP MGX KRE ROU 8TW 29G+11.8G(4008652)</t>
+          <t>470MM HM SHEET 4008115</t>
         </is>
       </c>
     </row>
@@ -516,27 +516,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10.000</t>
+          <t>26.210</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.08</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.56</t>
+          <t>0.9</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>9.240</t>
+          <t>25.230</t>
         </is>
       </c>
     </row>
@@ -546,27 +546,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>31</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>12.000</t>
+          <t>27.480</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.08</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.56</t>
+          <t>0.9</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>11.240</t>
+          <t>26.500</t>
         </is>
       </c>
     </row>
@@ -576,27 +576,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>32</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14.000</t>
+          <t>33.530</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.08</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.56</t>
+          <t>0.9</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>13.240</t>
+          <t>32.550</t>
         </is>
       </c>
     </row>
@@ -606,228 +606,48 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>33</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>15.000</t>
+          <t>26.360</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.08</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.56</t>
+          <t>0.9</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>14.240</t>
+          <t>25.380</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>5</v>
-      </c>
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>16.000</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0.56</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>15.240</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>6</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1234.000</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0.56</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>1233.240</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>7</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>225.000</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0.56</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>224.240</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>8</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>125.000</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>0.56</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>124.240</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>9</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1258.000</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>0.56</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>1257.240</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>10</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2244.000</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0.56</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2243.240</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>5153</v>
-      </c>
-      <c r="D16" t="n">
-        <v>2</v>
-      </c>
-      <c r="E16" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="F16" t="n">
-        <v>5145.4</v>
+      <c r="C10" t="n">
+        <v>113.58</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="F10" t="n">
+        <v>109.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>